<commit_message>
update ML model in attempt to decode
</commit_message>
<xml_diff>
--- a/references/Dictionary 6 - RPA Only Rejections.xlsx
+++ b/references/Dictionary 6 - RPA Only Rejections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpashayan\PycharmProjects\Monthly_Audit_2023\Monthly-Audit-2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpashayan\PycharmProjects\Monthly_Audit\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88AEAF9F-D518-4FA4-B8B6-B59DA7D94100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33951C3D-0027-4696-A8DA-71C49ADACACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BD92FB04-E732-4131-9530-A8F05553D04A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{BD92FB04-E732-4131-9530-A8F05553D04A}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary 6 - RPA Only" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
   <si>
     <t>Code</t>
   </si>
@@ -250,27 +250,6 @@
   </si>
   <si>
     <t>RPA-SPNI HDX No response</t>
-  </si>
-  <si>
-    <t>RPA200</t>
-  </si>
-  <si>
-    <t>RPA201</t>
-  </si>
-  <si>
-    <t>RPA202</t>
-  </si>
-  <si>
-    <t>RPA-TD Records Saved to Mdrive</t>
-  </si>
-  <si>
-    <t>HF $0 MR</t>
-  </si>
-  <si>
-    <t>RPA-TD Records Could Not Be found</t>
-  </si>
-  <si>
-    <t>RPA-Records Submitted To Carrier</t>
   </si>
   <si>
     <t>Bot Name</t>
@@ -292,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -308,12 +287,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -338,15 +311,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -386,8 +353,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD6928A9-4F7D-4763-8A59-593B9EF59BBE}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D33" xr:uid="{BD6928A9-4F7D-4763-8A59-593B9EF59BBE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD6928A9-4F7D-4763-8A59-593B9EF59BBE}" name="Table1" displayName="Table1" ref="A1:D30" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D30" xr:uid="{BD6928A9-4F7D-4763-8A59-593B9EF59BBE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{804BCC13-17E7-4155-922E-1994FD073D25}" name="Code" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{D2777DE4-FD13-4E36-A35E-BD9EB81D61AA}" name="Name" dataDxfId="2"/>
@@ -695,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28004EA-32BF-4A9C-AEC5-6FFD741633D9}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -723,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -736,8 +703,8 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>79</v>
+      <c r="D2" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -793,7 +760,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -821,7 +788,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -835,7 +802,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -849,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -862,8 +829,8 @@
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>79</v>
+      <c r="D11" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -876,8 +843,8 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>79</v>
+      <c r="D12" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -961,7 +928,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -975,7 +942,7 @@
         <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -989,7 +956,7 @@
         <v>43</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1130,39 +1097,6 @@
       </c>
       <c r="D30" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>